<commit_message>
[New] Added comparative results and files
</commit_message>
<xml_diff>
--- a/validation_assay_large/Compare_CEMchrR_VISPA2-GDB.forPaper.xlsx
+++ b/validation_assay_large/Compare_CEMchrR_VISPA2-GDB.forPaper.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calabria.andrea/Dropbox (HSR Global)/TIGET/Docs/Publications/Paper/WIP 2022 GraphDB/GigaScience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fvl58-my.sharepoint.com/personal/acalabria_tesseratx_com/Documents/Utils/GitHub/InCliniGene/validation_assay_large/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCCC808-4D44-2841-A235-E1936BCCBC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7DCCC808-4D44-2841-A235-E1936BCCBC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEA490FA-9484-6C4F-9112-D774E7A691E7}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="6200" windowWidth="22380" windowHeight="20160" xr2:uid="{307CA982-93CC-1746-A8C0-05BBB1DE5491}"/>
+    <workbookView xWindow="10420" yWindow="6200" windowWidth="22380" windowHeight="20160" activeTab="1" xr2:uid="{307CA982-93CC-1746-A8C0-05BBB1DE5491}"/>
   </bookViews>
   <sheets>
     <sheet name="VISPA2" sheetId="1" r:id="rId1"/>
     <sheet name="gTRIS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -152,9 +152,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -164,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -186,6 +195,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799C90CE-B27C-2540-B2A5-29A42519D1C8}">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3624,7 +3636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0D3E30-C65C-4A45-AD81-2497F0CBE725}">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -3747,7 +3759,7 @@
       <c r="H4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="8">
         <v>8.4766775143344208</v>
       </c>
     </row>

</xml_diff>